<commit_message>
DB Connection and Assessment Report from Query and Export Data as excel
</commit_message>
<xml_diff>
--- a/Assignement sheet.xlsx
+++ b/Assignement sheet.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A81F4D9-5132-435D-A6A1-D6F1C59EB47D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{FEFAA6F0-E06A-46C1-807F-71DC7ED207DB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" r:id="rId1"/>
@@ -28,7 +22,7 @@
     <sheet name="foreign_key_constraint" sheetId="13" r:id="rId13"/>
     <sheet name="user_table" sheetId="2" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -205,7 +199,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -235,7 +229,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -297,7 +292,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -349,7 +344,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -543,25 +538,25 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ED4B318-89CC-4112-9B28-2F3028BEE85D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -796,72 +791,72 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28870246-24D9-436F-AE24-2491BEAF837A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50837E85-A168-4368-8170-C3B74711A75D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB452E2F-EB7B-4E00-9256-A2C15B8A2AE2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FF0960-E147-40BE-8E1E-A9B133180DC3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C089DC31-098E-4B91-9262-A9BC28909683}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -869,21 +864,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BECF53-6471-4292-A9C3-CB19AF373864}">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AC16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" customWidth="1"/>
     <col min="5" max="5" width="53" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -896,11 +891,35 @@
       <c r="D1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -913,11 +932,35 @@
       <c r="D2" t="s">
         <v>34</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -930,11 +973,35 @@
       <c r="D3" t="s">
         <v>34</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -947,11 +1014,35 @@
       <c r="D4" t="s">
         <v>34</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -964,8 +1055,33 @@
       <c r="D5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -978,11 +1094,35 @@
       <c r="D6" t="s">
         <v>34</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -995,11 +1135,35 @@
       <c r="D7" t="s">
         <v>34</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1012,11 +1176,35 @@
       <c r="D8" t="s">
         <v>34</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1029,8 +1217,33 @@
       <c r="D9" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="1"/>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1043,11 +1256,35 @@
       <c r="D10" t="s">
         <v>34</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1060,11 +1297,35 @@
       <c r="D11" t="s">
         <v>34</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1077,11 +1338,35 @@
       <c r="D12" t="s">
         <v>34</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="1"/>
+      <c r="AC12" s="1"/>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1094,11 +1379,35 @@
       <c r="D13" t="s">
         <v>34</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="1"/>
+      <c r="AC13" s="1"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1111,11 +1420,35 @@
       <c r="D14" t="s">
         <v>34</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1"/>
+      <c r="AC14" s="1"/>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1128,8 +1461,33 @@
       <c r="D15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="1"/>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -1142,24 +1500,66 @@
       <c r="D16" t="s">
         <v>34</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="1"/>
+      <c r="AC16" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="E6:AC6"/>
+    <mergeCell ref="E1:AC1"/>
+    <mergeCell ref="E2:AC2"/>
+    <mergeCell ref="E3:AC3"/>
+    <mergeCell ref="E4:AC4"/>
+    <mergeCell ref="E5:AC5"/>
+    <mergeCell ref="E13:AC13"/>
+    <mergeCell ref="E14:AC14"/>
+    <mergeCell ref="E15:AC15"/>
+    <mergeCell ref="E16:AC16"/>
+    <mergeCell ref="E7:AC7"/>
+    <mergeCell ref="E8:AC8"/>
+    <mergeCell ref="E9:AC9"/>
+    <mergeCell ref="E10:AC10"/>
+    <mergeCell ref="E11:AC11"/>
+    <mergeCell ref="E12:AC12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BADC9D53-95BD-49E1-AA71-BE606C7BF4A9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1172,28 +1572,28 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F089A821-BB0B-494D-B55D-070EF00A30C2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4981449E-EE83-4AB8-BC80-8E5273E88F6A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1206,56 +1606,56 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B92DC2C-ADA1-4C32-913C-BA4D9FCCE1D8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F8680A4-CF1C-433E-9704-378555A35884}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBAC9701-343F-4FE9-BE45-AD7BA85A201E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC59571D-32DE-4617-AA5C-D0F1E26DE726}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>